<commit_message>
Added sensitivity analysis for C and k, changed some older titrant molinity scripts
</commit_message>
<xml_diff>
--- a/logbook_in_situ_corrected.xlsx
+++ b/logbook_in_situ_corrected.xlsx
@@ -1,21 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0e67038fc02b579b/Documenten/GitHub/tidegas/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13" documentId="11_1A65FAB5967F8CDEE54878D6425DCE3A874FB5F0" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1166DCBC-C605-4DF3-9179-0CD9154F52E8}"/>
+  <xr:revisionPtr revIDLastSave="14" documentId="11_1A65FAB5967F8CDEE54878D6425DCE3A874FB5F0" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3DA8363D-4810-43F1-B355-9C95A4837CEF}"/>
   <bookViews>
-    <workbookView xWindow="29715" yWindow="915" windowWidth="21600" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -2369,8 +2382,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AQ339"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E55" workbookViewId="0">
-      <selection activeCell="Y34" sqref="Y34"/>
+    <sheetView tabSelected="1" topLeftCell="D6" workbookViewId="0">
+      <selection activeCell="T6" sqref="T1:T1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4330,7 +4343,7 @@
         <v>1650.4814576741401</v>
       </c>
       <c r="T29">
-        <v>1730.039642733524</v>
+        <v>1728.4111633839241</v>
       </c>
       <c r="V29">
         <v>0</v>
@@ -4419,7 +4432,7 @@
         <v>1867.2677651954241</v>
       </c>
       <c r="T30">
-        <v>1940.575616347631</v>
+        <v>1939.0750753074369</v>
       </c>
       <c r="V30">
         <v>0</v>
@@ -4493,7 +4506,7 @@
         <v>2086.960593651359</v>
       </c>
       <c r="T31">
-        <v>2126.8574615062348</v>
+        <v>2126.0408110840708</v>
       </c>
       <c r="V31">
         <v>0</v>
@@ -4582,7 +4595,7 @@
         <v>1768.674938691129</v>
       </c>
       <c r="T32">
-        <v>1853.9812475495039</v>
+        <v>1852.235109647253</v>
       </c>
       <c r="V32">
         <v>0</v>
@@ -4671,7 +4684,7 @@
         <v>1684.514500298744</v>
       </c>
       <c r="T33">
-        <v>1765.727793365797</v>
+        <v>1764.065435550898</v>
       </c>
       <c r="V33">
         <v>0</v>
@@ -4760,7 +4773,7 @@
         <v>1566.6935672443669</v>
       </c>
       <c r="T34">
-        <v>1642.1761690609919</v>
+        <v>1640.6311129712799</v>
       </c>
       <c r="V34">
         <v>0</v>
@@ -4929,7 +4942,7 @@
         <v>1626.0041952186909</v>
       </c>
       <c r="T36">
-        <v>1704.3772093391281</v>
+        <v>1702.772989296077</v>
       </c>
       <c r="V36">
         <v>0</v>
@@ -5030,7 +5043,7 @@
         <v>1887.7676925448279</v>
       </c>
       <c r="T37">
-        <v>1974.2544363632601</v>
+        <v>1972.4841360953819</v>
       </c>
       <c r="V37">
         <v>0</v>
@@ -5122,7 +5135,7 @@
         <v>2073.6655701738082</v>
       </c>
       <c r="T38">
-        <v>2119.7915473007092</v>
+        <v>2118.847393016958</v>
       </c>
       <c r="V38">
         <v>0</v>
@@ -5211,7 +5224,7 @@
         <v>2022.103396683485</v>
       </c>
       <c r="T39">
-        <v>2079.9311030951558</v>
+        <v>2078.7387755524251</v>
       </c>
       <c r="V39">
         <v>0.5</v>
@@ -5300,7 +5313,7 @@
         <v>2071.4397525288991</v>
       </c>
       <c r="T40">
-        <v>2117.457452082986</v>
+        <v>2116.5155141367659</v>
       </c>
       <c r="V40">
         <v>0</v>
@@ -5389,7 +5402,7 @@
         <v>1906.5536530976669</v>
       </c>
       <c r="T41">
-        <v>1993.9542625314079</v>
+        <v>1992.1652563154039</v>
       </c>
       <c r="V41">
         <v>0</v>
@@ -5481,7 +5494,7 @@
         <v>1897.699863135228</v>
       </c>
       <c r="T42">
-        <v>1984.6697693217709</v>
+        <v>1982.8895791860141</v>
       </c>
       <c r="V42">
         <v>0</v>
@@ -5573,7 +5586,7 @@
         <v>1892.8755347947681</v>
       </c>
       <c r="T43">
-        <v>1979.6107557345861</v>
+        <v>1977.83536937958</v>
       </c>
       <c r="V43">
         <v>0</v>
@@ -5665,7 +5678,7 @@
         <v>1761.999410777345</v>
       </c>
       <c r="T44">
-        <v>1846.987381320771</v>
+        <v>1845.2477594969309</v>
       </c>
       <c r="V44">
         <v>0</v>
@@ -5757,7 +5770,7 @@
         <v>1776.503863913513</v>
       </c>
       <c r="T45">
-        <v>1862.197421001355</v>
+        <v>1860.4433565011759</v>
       </c>
       <c r="V45">
         <v>0</v>
@@ -5852,7 +5865,7 @@
         <v>1655.9529638285719</v>
       </c>
       <c r="T46">
-        <v>1735.78287177014</v>
+        <v>1734.1488305150981</v>
       </c>
       <c r="V46">
         <v>0</v>
@@ -5956,7 +5969,7 @@
         <v>1668.6995395236229</v>
       </c>
       <c r="T47">
-        <v>1749.14951995006</v>
+        <v>1747.5027864090371</v>
       </c>
       <c r="V47">
         <v>0</v>
@@ -6634,7 +6647,7 @@
         <v>519.2969954085205</v>
       </c>
       <c r="T56">
-        <v>1770.326543062273</v>
+        <v>1727.0774261756301</v>
       </c>
       <c r="V56">
         <v>40</v>
@@ -6729,7 +6742,7 @@
         <v>941.52255186799005</v>
       </c>
       <c r="T57">
-        <v>1785.1959247904931</v>
+        <v>1762.4220047633039</v>
       </c>
       <c r="V57">
         <v>20</v>
@@ -6830,7 +6843,7 @@
         <v>1284.798591662676</v>
       </c>
       <c r="T58">
-        <v>1812.3557636036301</v>
+        <v>1799.9086993448341</v>
       </c>
       <c r="V58">
         <v>10</v>
@@ -6934,7 +6947,7 @@
         <v>1473.45523177103</v>
       </c>
       <c r="T59">
-        <v>1791.873983586883</v>
+        <v>1784.869886623304</v>
       </c>
       <c r="V59">
         <v>5</v>
@@ -7038,7 +7051,7 @@
         <v>1597.712099691973</v>
       </c>
       <c r="T60">
-        <v>1777.3149702751721</v>
+        <v>1773.5304510336</v>
       </c>
       <c r="V60">
         <v>2</v>
@@ -7139,7 +7152,7 @@
         <v>1650.7734964102481</v>
       </c>
       <c r="T61">
-        <v>1756.260180118501</v>
+        <v>1754.085190201361</v>
       </c>
       <c r="V61">
         <v>0.5</v>
@@ -7243,7 +7256,7 @@
         <v>1690.321539871919</v>
       </c>
       <c r="T62">
-        <v>1771.8107865933939</v>
+        <v>1770.142780273223</v>
       </c>
       <c r="V62">
         <v>0</v>
@@ -7344,7 +7357,7 @@
         <v>1620.840478326307</v>
       </c>
       <c r="T63">
-        <v>1750.228141943762</v>
+        <v>1747.5409012868411</v>
       </c>
       <c r="V63">
         <v>1</v>
@@ -7448,7 +7461,7 @@
         <v>1222.8782374366219</v>
       </c>
       <c r="T64">
-        <v>1724.793054975856</v>
+        <v>1712.9509906108369</v>
       </c>
       <c r="V64">
         <v>10</v>
@@ -7543,7 +7556,7 @@
         <v>907.34790259621889</v>
       </c>
       <c r="T65">
-        <v>1720.0872581446381</v>
+        <v>1698.1483636858829</v>
       </c>
       <c r="V65">
         <v>20</v>
@@ -7647,7 +7660,7 @@
         <v>1408.287301662589</v>
       </c>
       <c r="T66">
-        <v>1712.522184194411</v>
+        <v>1705.8300826620609</v>
       </c>
       <c r="V66">
         <v>5</v>
@@ -7751,7 +7764,7 @@
         <v>470.94866924084369</v>
       </c>
       <c r="T67">
-        <v>1752.0214662659801</v>
+        <v>1706.171345967027</v>
       </c>
       <c r="V67">
         <v>43</v>
@@ -7855,7 +7868,7 @@
         <v>49.543318047040117</v>
       </c>
       <c r="T68">
-        <v>2432.6251534320468</v>
+        <v>2235.7270752876379</v>
       </c>
       <c r="V68">
         <v>140</v>
@@ -7956,7 +7969,7 @@
         <v>1631.057245848632</v>
       </c>
       <c r="T69">
-        <v>1709.673701856975</v>
+        <v>1708.0644987931701</v>
       </c>
       <c r="V69">
         <v>0</v>
@@ -8057,7 +8070,7 @@
         <v>1028.2501101673629</v>
       </c>
       <c r="T70">
-        <v>1706.599562287809</v>
+        <v>1689.3489301596831</v>
       </c>
       <c r="V70">
         <v>15.5</v>
@@ -8161,7 +8174,7 @@
         <v>1618.8740616398741</v>
       </c>
       <c r="T71">
-        <v>1722.315585271215</v>
+        <v>1720.1827637339111</v>
       </c>
       <c r="V71">
         <v>0.5</v>
@@ -8256,7 +8269,7 @@
         <v>916.10764003575002</v>
       </c>
       <c r="T72">
-        <v>1736.806133039519</v>
+        <v>1714.6523915016569</v>
       </c>
       <c r="V72">
         <v>20</v>
@@ -8422,7 +8435,7 @@
         <v>1979.8620241908161</v>
       </c>
       <c r="T74">
-        <v>2078.5384999008638</v>
+        <v>2076.5172146505452</v>
       </c>
       <c r="V74">
         <v>0.05</v>
@@ -8496,7 +8509,7 @@
         <v>1874.3021460594739</v>
       </c>
       <c r="T75">
-        <v>2085.316886425308</v>
+        <v>2080.8704689344481</v>
       </c>
       <c r="V75">
         <v>2</v>
@@ -8570,7 +8583,7 @@
         <v>1713.0404122799971</v>
       </c>
       <c r="T76">
-        <v>2083.8145481631841</v>
+        <v>2075.658816176599</v>
       </c>
       <c r="V76">
         <v>5</v>
@@ -8644,7 +8657,7 @@
         <v>1275.6867749456439</v>
       </c>
       <c r="T77">
-        <v>2119.6712199535418</v>
+        <v>2098.2084397638018</v>
       </c>
       <c r="V77">
         <v>15.5</v>
@@ -8718,7 +8731,7 @@
         <v>370.2442420154203</v>
       </c>
       <c r="T78">
-        <v>2268.6923314084611</v>
+        <v>2186.9378101158668</v>
       </c>
       <c r="V78">
         <v>60</v>
@@ -8792,7 +8805,7 @@
         <v>1459.70560393812</v>
       </c>
       <c r="T79">
-        <v>2090.9259781402311</v>
+        <v>2075.9298813237019</v>
       </c>
       <c r="V79">
         <v>10.5</v>
@@ -8866,7 +8879,7 @@
         <v>1557.6649094049001</v>
       </c>
       <c r="T80">
-        <v>2102.5952014277391</v>
+        <v>2090.0033292014641</v>
       </c>
       <c r="V80">
         <v>8.5</v>
@@ -8940,7 +8953,7 @@
         <v>978.52346872940348</v>
       </c>
       <c r="T81">
-        <v>2154.0168069085348</v>
+        <v>2120.1700026324311</v>
       </c>
       <c r="V81">
         <v>25</v>
@@ -9014,7 +9027,7 @@
         <v>642.68570797766438</v>
       </c>
       <c r="T82">
-        <v>2266.9439224754728</v>
+        <v>2210.1353634709649</v>
       </c>
       <c r="V82">
         <v>41</v>
@@ -9088,7 +9101,7 @@
         <v>755.35171282992155</v>
       </c>
       <c r="T83">
-        <v>1924.567788316177</v>
+        <v>1888.7220330848729</v>
       </c>
       <c r="V83">
         <v>30</v>
@@ -9162,7 +9175,7 @@
         <v>1711.261426091407</v>
       </c>
       <c r="T84">
-        <v>2081.6471148877772</v>
+        <v>2073.4999273761809</v>
       </c>
       <c r="V84">
         <v>5</v>
@@ -9236,7 +9249,7 @@
         <v>1972.8207635809879</v>
       </c>
       <c r="T85">
-        <v>2068.0617088749618</v>
+        <v>2066.1122185424229</v>
       </c>
       <c r="V85">
         <v>0</v>
@@ -9316,7 +9329,7 @@
         <v>1664.8337513455481</v>
       </c>
       <c r="T86">
-        <v>1745.0801372895819</v>
+        <v>1743.437571131338</v>
       </c>
       <c r="V86">
         <v>0</v>
@@ -9414,7 +9427,7 @@
         <v>2091.9315153632419</v>
       </c>
       <c r="T87">
-        <v>2140.297461391252</v>
+        <v>2139.3074571035509</v>
       </c>
       <c r="V87">
         <v>0</v>
@@ -9506,7 +9519,7 @@
         <v>1231.649717421521</v>
       </c>
       <c r="T88">
-        <v>2178.0203011440171</v>
+        <v>2133.8451916908102</v>
       </c>
       <c r="V88">
         <v>68</v>
@@ -9598,7 +9611,7 @@
         <v>1931.1600302533141</v>
       </c>
       <c r="T89">
-        <v>2113.1501972527899</v>
+        <v>2109.1470511792209</v>
       </c>
       <c r="V89">
         <v>5</v>
@@ -9687,7 +9700,7 @@
         <v>2087.0161498770522</v>
       </c>
       <c r="T90">
-        <v>2135.1429820470371</v>
+        <v>2134.1578721894898</v>
       </c>
       <c r="V90">
         <v>0</v>
@@ -9779,7 +9792,7 @@
         <v>1955.2538445729349</v>
       </c>
       <c r="T91">
-        <v>2142.50496977591</v>
+        <v>2138.3861010535688</v>
       </c>
       <c r="V91">
         <v>5</v>
@@ -9871,7 +9884,7 @@
         <v>1860.638106826947</v>
       </c>
       <c r="T92">
-        <v>2177.6605107824071</v>
+        <v>2170.180756087776</v>
       </c>
       <c r="V92">
         <v>10</v>
@@ -9963,7 +9976,7 @@
         <v>1858.548438303626</v>
       </c>
       <c r="T93">
-        <v>2174.7025341865201</v>
+        <v>2167.2432661556109</v>
       </c>
       <c r="V93">
         <v>10</v>
@@ -10557,7 +10570,7 @@
         <v>1659.191118674499</v>
       </c>
       <c r="T102">
-        <v>1765.235103337857</v>
+        <v>1763.0486226437249</v>
       </c>
       <c r="V102">
         <v>0.5</v>
@@ -10652,7 +10665,7 @@
         <v>2064.013358805114</v>
       </c>
       <c r="T103">
-        <v>2111.25430267096</v>
+        <v>2110.2873260929532</v>
       </c>
       <c r="V103">
         <v>0</v>
@@ -10741,7 +10754,7 @@
         <v>2018.2685254714979</v>
       </c>
       <c r="T104">
-        <v>2123.289321517093</v>
+        <v>2121.0763656656131</v>
       </c>
       <c r="V104">
         <v>2</v>
@@ -10830,7 +10843,7 @@
         <v>2036.1965195219229</v>
       </c>
       <c r="T105">
-        <v>2143.25197904376</v>
+        <v>2140.9961495842408</v>
       </c>
       <c r="V105">
         <v>2</v>
@@ -10919,7 +10932,7 @@
         <v>1956.3486523672229</v>
       </c>
       <c r="T106">
-        <v>2144.885168877634</v>
+        <v>2140.738026049884</v>
       </c>
       <c r="V106">
         <v>5</v>
@@ -11008,7 +11021,7 @@
         <v>1199.187251965875</v>
       </c>
       <c r="T107">
-        <v>2321.5112156428572</v>
+        <v>2262.8189410786222</v>
       </c>
       <c r="V107">
         <v>80</v>
@@ -11097,7 +11110,7 @@
         <v>1657.2997554756939</v>
       </c>
       <c r="T108">
-        <v>2171.3307270806658</v>
+        <v>2157.4550962802318</v>
       </c>
       <c r="V108">
         <v>20</v>
@@ -11186,7 +11199,7 @@
         <v>1342.003728883004</v>
       </c>
       <c r="T109">
-        <v>2263.6119176511711</v>
+        <v>2227.9333775045179</v>
       </c>
       <c r="V109">
         <v>50</v>
@@ -11275,7 +11288,7 @@
         <v>1376.1412122209269</v>
       </c>
       <c r="T110">
-        <v>2238.6298446982528</v>
+        <v>2207.050096666389</v>
       </c>
       <c r="V110">
         <v>45</v>
@@ -11364,7 +11377,7 @@
         <v>1842.654907079527</v>
       </c>
       <c r="T111">
-        <v>2154.1960255072559</v>
+        <v>2146.8455950201478</v>
       </c>
       <c r="V111">
         <v>10</v>
@@ -11592,7 +11605,7 @@
         <v>2158.5445340951992</v>
       </c>
       <c r="T114">
-        <v>2182.5818057191109</v>
+        <v>2182.0897859422521</v>
       </c>
       <c r="V114">
         <v>0</v>
@@ -11681,7 +11694,7 @@
         <v>2076.0793341004378</v>
       </c>
       <c r="T115">
-        <v>2165.9663672539691</v>
+        <v>2163.989167442759</v>
       </c>
       <c r="V115">
         <v>5</v>
@@ -11770,7 +11783,7 @@
         <v>2095.9063383438552</v>
       </c>
       <c r="T116">
-        <v>2190.1226586431021</v>
+        <v>2188.0502296822938</v>
       </c>
       <c r="V116">
         <v>5</v>
@@ -11859,7 +11872,7 @@
         <v>2036.525324980377</v>
       </c>
       <c r="T117">
-        <v>2191.144049562452</v>
+        <v>2187.496010443951</v>
       </c>
       <c r="V117">
         <v>10</v>
@@ -11948,7 +11961,7 @@
         <v>1747.940077757336</v>
       </c>
       <c r="T118">
-        <v>2379.6362295444251</v>
+        <v>2349.568037690859</v>
       </c>
       <c r="V118">
         <v>70</v>
@@ -12037,7 +12050,7 @@
         <v>1944.504145263088</v>
       </c>
       <c r="T119">
-        <v>2215.891258056311</v>
+        <v>2208.469223095869</v>
       </c>
       <c r="V119">
         <v>21</v>
@@ -12126,7 +12139,7 @@
         <v>1886.7613967502889</v>
       </c>
       <c r="T120">
-        <v>2237.8944971310239</v>
+        <v>2227.1294799252669</v>
       </c>
       <c r="V120">
         <v>30</v>
@@ -12215,7 +12228,7 @@
         <v>2137.7628988966112</v>
       </c>
       <c r="T121">
-        <v>2175.9059101071198</v>
+        <v>2175.1137213648808</v>
       </c>
       <c r="V121">
         <v>1</v>
@@ -12304,7 +12317,7 @@
         <v>2124.5246454732501</v>
       </c>
       <c r="T122">
-        <v>2176.7422947634132</v>
+        <v>2175.6419855208792</v>
       </c>
       <c r="V122">
         <v>2</v>
@@ -12393,7 +12406,7 @@
         <v>2141.095284601849</v>
       </c>
       <c r="T123">
-        <v>2175.6581278694789</v>
+        <v>2174.9428955531098</v>
       </c>
       <c r="V123">
         <v>0.75</v>
@@ -12482,7 +12495,7 @@
         <v>2112.2721197872029</v>
       </c>
       <c r="T124">
-        <v>2178.286256449142</v>
+        <v>2176.8750660763098</v>
       </c>
       <c r="V124">
         <v>3</v>
@@ -12571,7 +12584,7 @@
         <v>1793.2179146374931</v>
       </c>
       <c r="T125">
-        <v>2307.1619790561508</v>
+        <v>2286.8264757218631</v>
       </c>
       <c r="V125">
         <v>52</v>
@@ -12660,7 +12673,7 @@
         <v>2145.530791869186</v>
       </c>
       <c r="T126">
-        <v>2168.5572327928448</v>
+        <v>2168.0859037459222</v>
       </c>
       <c r="V126">
         <v>0</v>
@@ -12752,7 +12765,7 @@
         <v>1683.629761408379</v>
       </c>
       <c r="T127">
-        <v>1791.2277542637869</v>
+        <v>1789.009232064225</v>
       </c>
       <c r="V127">
         <v>0.5</v>
@@ -12844,7 +12857,7 @@
         <v>1679.1615357529829</v>
       </c>
       <c r="T128">
-        <v>1786.471352812423</v>
+        <v>1784.258772400284</v>
       </c>
       <c r="V128">
         <v>0.5</v>
@@ -13013,7 +13026,7 @@
         <v>1721.4546049575531</v>
       </c>
       <c r="T130">
-        <v>1804.463167994277</v>
+        <v>1802.764062733839</v>
       </c>
       <c r="V130">
         <v>0</v>
@@ -14391,7 +14404,7 @@
         <v>1657.47881326588</v>
       </c>
       <c r="T147">
-        <v>1737.3726357061539</v>
+        <v>1735.7372861829399</v>
       </c>
       <c r="V147">
         <v>0</v>
@@ -14489,7 +14502,7 @@
         <v>1688.8106753165389</v>
       </c>
       <c r="T148">
-        <v>1774.624569313781</v>
+        <v>1772.8659065072859</v>
       </c>
       <c r="V148">
         <v>8.3330000000000001E-2</v>
@@ -14593,7 +14606,7 @@
         <v>1795.9627660196591</v>
       </c>
       <c r="T149">
-        <v>1882.595747200189</v>
+        <v>1880.822453594491</v>
       </c>
       <c r="V149">
         <v>0</v>
@@ -14685,7 +14698,7 @@
         <v>1847.5906500963131</v>
       </c>
       <c r="T150">
-        <v>1936.734435414148</v>
+        <v>1934.9097480683149</v>
       </c>
       <c r="V150">
         <v>0</v>
@@ -14777,7 +14790,7 @@
         <v>1923.4982392794029</v>
       </c>
       <c r="T151">
-        <v>2021.332036944003</v>
+        <v>2019.3270391437679</v>
       </c>
       <c r="V151">
         <v>8.3333000000000004E-2</v>
@@ -14854,7 +14867,7 @@
         <v>1990.07555459323</v>
       </c>
       <c r="T152">
-        <v>2075.369307114343</v>
+        <v>2073.623426228211</v>
       </c>
       <c r="V152">
         <v>0</v>
@@ -14946,7 +14959,7 @@
         <v>2046.183997506331</v>
       </c>
       <c r="T153">
-        <v>2119.805409479904</v>
+        <v>2118.2984501519868</v>
       </c>
       <c r="V153">
         <v>0</v>
@@ -15041,7 +15054,7 @@
         <v>2074.647136571708</v>
       </c>
       <c r="T154">
-        <v>2142.0056345325229</v>
+        <v>2140.623517699742</v>
       </c>
       <c r="V154">
         <v>0.16666600000000001</v>
@@ -15136,7 +15149,7 @@
         <v>2088.176085101496</v>
       </c>
       <c r="T155">
-        <v>2171.9578263640519</v>
+        <v>2170.2135607426608</v>
       </c>
       <c r="V155">
         <v>1.166666</v>
@@ -15231,7 +15244,7 @@
         <v>2110.2330978930599</v>
       </c>
       <c r="T156">
-        <v>2158.6982660725162</v>
+        <v>2157.7062308030299</v>
       </c>
       <c r="V156">
         <v>0</v>
@@ -15326,7 +15339,7 @@
         <v>2181.8628742164419</v>
       </c>
       <c r="T157">
-        <v>2206.0943384211309</v>
+        <v>2205.598343709356</v>
       </c>
       <c r="V157">
         <v>0</v>
@@ -15418,7 +15431,7 @@
         <v>2236.5688366296481</v>
       </c>
       <c r="T158">
-        <v>2242.9484930280369</v>
+        <v>2242.81790761191</v>
       </c>
       <c r="V158">
         <v>0</v>
@@ -15495,7 +15508,7 @@
         <v>2225.4638251201281</v>
       </c>
       <c r="T159">
-        <v>2224.5084091131221</v>
+        <v>2224.527965557711</v>
       </c>
       <c r="V159">
         <v>0</v>
@@ -15572,7 +15585,7 @@
         <v>2100.823263153713</v>
       </c>
       <c r="T160">
-        <v>2041.742804314023</v>
+        <v>2045.002887320293</v>
       </c>
       <c r="V160">
         <v>86</v>
@@ -15649,7 +15662,7 @@
         <v>2232.4895447317422</v>
       </c>
       <c r="T161">
-        <v>2238.6707590760329</v>
+        <v>2238.5442355774439</v>
       </c>
       <c r="V161">
         <v>0</v>
@@ -16749,7 +16762,7 @@
         <v>1684.854397563249</v>
       </c>
       <c r="T174">
-        <v>1766.080403247478</v>
+        <v>1764.4177852175601</v>
       </c>
       <c r="V174">
         <v>0</v>
@@ -16921,7 +16934,7 @@
         <v>1648.4843633432961</v>
       </c>
       <c r="T176">
-        <v>1727.9411050280739</v>
+        <v>1726.3147021265549</v>
       </c>
       <c r="V176">
         <v>0</v>
@@ -17025,7 +17038,7 @@
         <v>1639.0246610764309</v>
       </c>
       <c r="T177">
-        <v>1718.021113805966</v>
+        <v>1716.4041325756159</v>
       </c>
       <c r="V177">
         <v>0</v>
@@ -17120,7 +17133,7 @@
         <v>1697.4083239164761</v>
       </c>
       <c r="T178">
-        <v>1779.244770751968</v>
+        <v>1777.569657580184</v>
       </c>
       <c r="V178">
         <v>0</v>
@@ -17215,7 +17228,7 @@
         <v>1756.480022268317</v>
       </c>
       <c r="T179">
-        <v>1841.1896558130679</v>
+        <v>1839.455731279259</v>
       </c>
       <c r="V179">
         <v>0</v>
@@ -17310,7 +17323,7 @@
         <v>1833.794616865149</v>
       </c>
       <c r="T180">
-        <v>1922.263868613484</v>
+        <v>1920.452988319531</v>
       </c>
       <c r="V180">
         <v>0</v>
@@ -17405,7 +17418,7 @@
         <v>1907.8041889899921</v>
       </c>
       <c r="T181">
-        <v>1996.3823622707871</v>
+        <v>1994.5692524580711</v>
       </c>
       <c r="V181">
         <v>0</v>
@@ -17485,7 +17498,7 @@
         <v>1963.4600262020181</v>
       </c>
       <c r="T182">
-        <v>2040.269224222734</v>
+        <v>2038.6970139876371</v>
       </c>
       <c r="V182">
         <v>0</v>
@@ -17580,7 +17593,7 @@
         <v>2017.0132263436319</v>
       </c>
       <c r="T183">
-        <v>2082.1423495102608</v>
+        <v>2080.8092191471778</v>
       </c>
       <c r="V183">
         <v>0</v>
@@ -17675,7 +17688,7 @@
         <v>2061.4349175264801</v>
       </c>
       <c r="T184">
-        <v>2114.610836578262</v>
+        <v>2113.5223767798489</v>
       </c>
       <c r="V184">
         <v>0</v>
@@ -17770,7 +17783,7 @@
         <v>2122.8382962162</v>
       </c>
       <c r="T185">
-        <v>2158.0993323687899</v>
+        <v>2157.3775729523691</v>
       </c>
       <c r="V185">
         <v>0</v>
@@ -18066,7 +18079,7 @@
         <v>1627.248074974648</v>
       </c>
       <c r="T189">
-        <v>1705.6969118298409</v>
+        <v>1704.091139768507</v>
       </c>
       <c r="V189">
         <v>0</v>
@@ -18170,7 +18183,7 @@
         <v>1642.571102457194</v>
       </c>
       <c r="T190">
-        <v>1721.7653463890899</v>
+        <v>1720.1443165635101</v>
       </c>
       <c r="V190">
         <v>0</v>
@@ -18274,7 +18287,7 @@
         <v>426.43183195248548</v>
       </c>
       <c r="T191">
-        <v>1680.467600937397</v>
+        <v>1634.5514785489329</v>
       </c>
       <c r="V191">
         <v>45</v>
@@ -18375,7 +18388,7 @@
         <v>1202.624744663914</v>
       </c>
       <c r="T192">
-        <v>1696.274783637381</v>
+        <v>1684.627716583296</v>
       </c>
       <c r="V192">
         <v>10</v>
@@ -18482,7 +18495,7 @@
         <v>1656.2242895971281</v>
       </c>
       <c r="T193">
-        <v>1736.0804231821171</v>
+        <v>1734.4458451134369</v>
       </c>
       <c r="V193">
         <v>0</v>
@@ -18583,7 +18596,7 @@
         <v>2142.6502762534669</v>
       </c>
       <c r="T194">
-        <v>2172.187214753857</v>
+        <v>2171.5826220980239</v>
       </c>
       <c r="V194">
         <v>0</v>
@@ -18675,7 +18688,7 @@
         <v>2209.8173523589412</v>
       </c>
       <c r="T195">
-        <v>2208.8865786049219</v>
+        <v>2208.905630646349</v>
       </c>
       <c r="V195">
         <v>0</v>
@@ -18755,7 +18768,7 @@
         <v>1531.4364062450279</v>
       </c>
       <c r="T196">
-        <v>1605.2654801677229</v>
+        <v>1603.7542701999059</v>
       </c>
       <c r="V196">
         <v>0</v>
@@ -18930,7 +18943,7 @@
         <v>1549.509856614337</v>
       </c>
       <c r="T198">
-        <v>1624.2181352386531</v>
+        <v>1622.688928798196</v>
       </c>
       <c r="V198">
         <v>0</v>
@@ -19170,7 +19183,7 @@
         <v>1636.15251142389</v>
       </c>
       <c r="T201">
-        <v>1715.0335335335869</v>
+        <v>1713.418915056744</v>
       </c>
       <c r="V201">
         <v>0</v>
@@ -19277,7 +19290,7 @@
         <v>1642.2351019334949</v>
       </c>
       <c r="T202">
-        <v>1721.4120189644609</v>
+        <v>1719.791343803839</v>
       </c>
       <c r="V202">
         <v>0</v>
@@ -19381,7 +19394,7 @@
         <v>1903.7877981578999</v>
       </c>
       <c r="T203">
-        <v>1991.619104154973</v>
+        <v>1989.821281995532</v>
       </c>
       <c r="V203">
         <v>0</v>
@@ -19461,7 +19474,7 @@
         <v>1727.0036606006499</v>
       </c>
       <c r="T204">
-        <v>1810.3039774372919</v>
+        <v>1808.5989002578369</v>
       </c>
       <c r="V204">
         <v>0</v>
@@ -19556,7 +19569,7 @@
         <v>1808.879335016343</v>
       </c>
       <c r="T205">
-        <v>1896.161864639477</v>
+        <v>1894.3752754033601</v>
       </c>
       <c r="V205">
         <v>0</v>
@@ -19651,7 +19664,7 @@
         <v>1892.5220260193059</v>
       </c>
       <c r="T206">
-        <v>1983.859507926669</v>
+        <v>1981.9899177264961</v>
       </c>
       <c r="V206">
         <v>0</v>
@@ -19731,7 +19744,7 @@
         <v>1970.090506669093</v>
       </c>
       <c r="T207">
-        <v>2046.85971648998</v>
+        <v>2045.288324774782</v>
       </c>
       <c r="V207">
         <v>0</v>
@@ -19823,7 +19836,7 @@
         <v>2208.7297223440492</v>
       </c>
       <c r="T208">
-        <v>2208.1367833366362</v>
+        <v>2208.1489202264911</v>
       </c>
       <c r="V208">
         <v>0</v>
@@ -19903,7 +19916,7 @@
         <v>2014.436759557394</v>
       </c>
       <c r="T209">
-        <v>2079.27894346111</v>
+        <v>2077.9516864681141</v>
       </c>
       <c r="V209">
         <v>0</v>
@@ -19998,7 +20011,7 @@
         <v>2084.0256601638471</v>
       </c>
       <c r="T210">
-        <v>2131.4528425966851</v>
+        <v>2130.482053894757</v>
       </c>
       <c r="V210">
         <v>0</v>
@@ -20093,7 +20106,7 @@
         <v>2083.549520132924</v>
       </c>
       <c r="T211">
-        <v>2130.953540162056</v>
+        <v>2129.9832255722008</v>
       </c>
       <c r="V211">
         <v>0</v>
@@ -20191,7 +20204,7 @@
         <v>1659.961540953321</v>
       </c>
       <c r="T212">
-        <v>1740.0007819020091</v>
+        <v>1738.3624558021199</v>
       </c>
       <c r="V212">
         <v>0</v>
@@ -20295,7 +20308,7 @@
         <v>2025.0427885111801</v>
       </c>
       <c r="T213">
-        <v>2090.4009154324799</v>
+        <v>2089.0630975833119</v>
       </c>
       <c r="V213">
         <v>0</v>
@@ -20390,7 +20403,7 @@
         <v>2111.3987318062532</v>
       </c>
       <c r="T214">
-        <v>2153.2983161633342</v>
+        <v>2152.4406720651</v>
       </c>
       <c r="V214">
         <v>0</v>
@@ -20485,7 +20498,7 @@
         <v>2126.143644109236</v>
       </c>
       <c r="T215">
-        <v>2161.933841967807</v>
+        <v>2161.2012511214061</v>
       </c>
       <c r="V215">
         <v>0</v>
@@ -20580,7 +20593,7 @@
         <v>2140.9179489777048</v>
       </c>
       <c r="T216">
-        <v>2170.630290742065</v>
+        <v>2170.022107750518</v>
       </c>
       <c r="V216">
         <v>0</v>
@@ -20675,7 +20688,7 @@
         <v>2157.801097182477</v>
       </c>
       <c r="T217">
-        <v>2181.5660349463928</v>
+        <v>2181.0795895811029</v>
       </c>
       <c r="V217">
         <v>0</v>
@@ -20770,7 +20783,7 @@
         <v>2171.3521853859138</v>
       </c>
       <c r="T218">
-        <v>2189.033424028145</v>
+        <v>2188.671506118847</v>
       </c>
       <c r="V218">
         <v>0</v>
@@ -20865,7 +20878,7 @@
         <v>2184.320146465373</v>
       </c>
       <c r="T219">
-        <v>2195.913198608393</v>
+        <v>2195.6759000073789</v>
       </c>
       <c r="V219">
         <v>0</v>
@@ -20957,7 +20970,7 @@
         <v>2196.0711939419489</v>
       </c>
       <c r="T220">
-        <v>2201.5389589179031</v>
+        <v>2201.4270390400789</v>
       </c>
       <c r="V220">
         <v>0</v>
@@ -21034,7 +21047,7 @@
         <v>2203.1856595352579</v>
       </c>
       <c r="T221">
-        <v>2202.323022933419</v>
+        <v>2202.3406802730292</v>
       </c>
       <c r="V221">
         <v>0</v>
@@ -21120,7 +21133,7 @@
         <v>1684.8624146541999</v>
       </c>
       <c r="T222">
-        <v>1766.112988513037</v>
+        <v>1764.44986759627</v>
       </c>
       <c r="V222">
         <v>0</v>
@@ -21330,7 +21343,7 @@
         <v>1648.281071743037</v>
       </c>
       <c r="T225">
-        <v>1727.7545411409551</v>
+        <v>1726.1277958392741</v>
       </c>
       <c r="V225">
         <v>0</v>
@@ -21422,7 +21435,7 @@
         <v>504.42584228665231</v>
       </c>
       <c r="T226">
-        <v>2458.9980169262531</v>
+        <v>2381.660400391173</v>
       </c>
       <c r="V226">
         <v>52</v>
@@ -21499,7 +21512,7 @@
         <v>1997.8042260852769</v>
       </c>
       <c r="T227">
-        <v>2094.27970461107</v>
+        <v>2092.304944573435</v>
       </c>
       <c r="V227">
         <v>0</v>
@@ -21576,7 +21589,7 @@
         <v>1515.5236294632839</v>
       </c>
       <c r="T228">
-        <v>2139.194969652192</v>
+        <v>2124.4802095075429</v>
       </c>
       <c r="V228">
         <v>10</v>
@@ -21653,7 +21666,7 @@
         <v>1796.630031535462</v>
       </c>
       <c r="T229">
-        <v>2121.5752903471948</v>
+        <v>2114.5287239757372</v>
       </c>
       <c r="V229">
         <v>4</v>
@@ -21730,7 +21743,7 @@
         <v>1741.377367975907</v>
       </c>
       <c r="T230">
-        <v>2150.2203519176492</v>
+        <v>2141.1632143872721</v>
       </c>
       <c r="V230">
         <v>5.5</v>
@@ -21807,7 +21820,7 @@
         <v>811.12265763710889</v>
       </c>
       <c r="T231">
-        <v>2196.0774472223688</v>
+        <v>2152.5605294461998</v>
       </c>
       <c r="V231">
         <v>32</v>
@@ -21884,7 +21897,7 @@
         <v>1137.7581437880369</v>
       </c>
       <c r="T232">
-        <v>2293.3924286350762</v>
+        <v>2261.3745396517688</v>
       </c>
       <c r="V232">
         <v>22</v>
@@ -21961,7 +21974,7 @@
         <v>1955.6514496195859</v>
       </c>
       <c r="T233">
-        <v>2112.0659189215089</v>
+        <v>2108.817360987257</v>
       </c>
       <c r="V233">
         <v>1</v>
@@ -22038,7 +22051,7 @@
         <v>1904.8285233467029</v>
       </c>
       <c r="T234">
-        <v>2119.3524814759412</v>
+        <v>2114.832119163902</v>
       </c>
       <c r="V234">
         <v>2</v>
@@ -22115,7 +22128,7 @@
         <v>1931.5536098066459</v>
       </c>
       <c r="T235">
-        <v>2117.3318591273178</v>
+        <v>2113.44539644919</v>
       </c>
       <c r="V235">
         <v>1.5</v>
@@ -22192,7 +22205,7 @@
         <v>2009.907842741585</v>
       </c>
       <c r="T236">
-        <v>2106.9721162375358</v>
+        <v>2104.9853041344941</v>
       </c>
       <c r="V236">
         <v>0</v>
@@ -22334,7 +22347,7 @@
         <v>891.44752086258109</v>
       </c>
       <c r="T238">
-        <v>2255.4979343708892</v>
+        <v>2193.692950369169</v>
       </c>
       <c r="V238">
         <v>65</v>
@@ -22411,7 +22424,7 @@
         <v>1147.0968611291789</v>
       </c>
       <c r="T239">
-        <v>2217.6333536815409</v>
+        <v>2181.4821736323311</v>
       </c>
       <c r="V239">
         <v>38</v>
@@ -22488,7 +22501,7 @@
         <v>271.10462841437283</v>
       </c>
       <c r="T240">
-        <v>2646.877845744069</v>
+        <v>2527.1411218953458</v>
       </c>
       <c r="V240">
         <v>76</v>
@@ -22565,7 +22578,7 @@
         <v>1544.634707198665</v>
       </c>
       <c r="T241">
-        <v>2103.7025086297972</v>
+        <v>2089.580488322877</v>
       </c>
       <c r="V241">
         <v>15</v>
@@ -22642,7 +22655,7 @@
         <v>2054.7051601710109</v>
       </c>
       <c r="T242">
-        <v>2128.9488517006971</v>
+        <v>2127.4254589599468</v>
       </c>
       <c r="V242">
         <v>0.16666</v>
@@ -22719,7 +22732,7 @@
         <v>2054.107275770486</v>
       </c>
       <c r="T243">
-        <v>2121.082198456375</v>
+        <v>2119.7112863565881</v>
       </c>
       <c r="V243">
         <v>0</v>
@@ -22796,7 +22809,7 @@
         <v>1973.36596429104</v>
       </c>
       <c r="T244">
-        <v>2120.454057793941</v>
+        <v>2117.3546768193469</v>
       </c>
       <c r="V244">
         <v>2</v>
@@ -22873,7 +22886,7 @@
         <v>1878.8226485859559</v>
       </c>
       <c r="T245">
-        <v>2141.1719745783821</v>
+        <v>2135.4012085443419</v>
       </c>
       <c r="V245">
         <v>5</v>
@@ -23077,7 +23090,7 @@
         <v>1634.056792784681</v>
       </c>
       <c r="T248">
-        <v>1712.8498552735689</v>
+        <v>1711.2370372453661</v>
       </c>
       <c r="V248">
         <v>0</v>
@@ -23175,7 +23188,7 @@
         <v>1646.405652777245</v>
       </c>
       <c r="T249">
-        <v>1725.7994403929499</v>
+        <v>1724.174326100534</v>
       </c>
       <c r="V249">
         <v>0</v>
@@ -23273,7 +23286,7 @@
         <v>937.50265460300716</v>
       </c>
       <c r="T250">
-        <v>1887.356236004797</v>
+        <v>1861.0396868001801</v>
       </c>
       <c r="V250">
         <v>22</v>
@@ -23368,7 +23381,7 @@
         <v>1203.7350021593099</v>
       </c>
       <c r="T251">
-        <v>1749.231267952433</v>
+        <v>1736.182162228429</v>
       </c>
       <c r="V251">
         <v>11</v>
@@ -23463,7 +23476,7 @@
         <v>1426.9786065476851</v>
       </c>
       <c r="T252">
-        <v>1752.729639891505</v>
+        <v>1745.5302759119991</v>
       </c>
       <c r="V252">
         <v>5.3333300000000001</v>
@@ -23561,7 +23574,7 @@
         <v>1594.921422821136</v>
       </c>
       <c r="T253">
-        <v>1774.302954110289</v>
+        <v>1770.5230988410381</v>
       </c>
       <c r="V253">
         <v>2</v>
@@ -23656,7 +23669,7 @@
         <v>1664.720528456932</v>
       </c>
       <c r="T254">
-        <v>1744.991103876034</v>
+        <v>1743.3480425825551</v>
       </c>
       <c r="V254">
         <v>0</v>
@@ -23745,7 +23758,7 @@
         <v>1651.5168650987171</v>
       </c>
       <c r="T255">
-        <v>1731.1451324545569</v>
+        <v>1729.5152185879119</v>
       </c>
       <c r="V255">
         <v>0</v>
@@ -23843,7 +23856,7 @@
         <v>1086.0597204386811</v>
       </c>
       <c r="T256">
-        <v>1724.6302417463969</v>
+        <v>1708.716264853753</v>
       </c>
       <c r="V256">
         <v>14</v>
@@ -23938,7 +23951,7 @@
         <v>1661.2633086498331</v>
       </c>
       <c r="T257">
-        <v>1741.365703458878</v>
+        <v>1739.7260846603519</v>
       </c>
       <c r="V257">
         <v>0</v>
@@ -24036,7 +24049,7 @@
         <v>1654.5339986527561</v>
       </c>
       <c r="T258">
-        <v>1786.6810240009399</v>
+        <v>1783.936474410365</v>
       </c>
       <c r="V258">
         <v>1</v>
@@ -24131,7 +24144,7 @@
         <v>1859.404418131717</v>
       </c>
       <c r="T259">
-        <v>1949.1414603694459</v>
+        <v>1947.304629626396</v>
       </c>
       <c r="V259">
         <v>0</v>
@@ -24214,7 +24227,7 @@
         <v>1836.790145931943</v>
       </c>
       <c r="T260">
-        <v>1935.0063165627321</v>
+        <v>1932.9910369035381</v>
       </c>
       <c r="V260">
         <v>0.16666</v>
@@ -24294,7 +24307,7 @@
         <v>1036.226504674888</v>
       </c>
       <c r="T261">
-        <v>1852.938885730028</v>
+        <v>1831.465713187971</v>
       </c>
       <c r="V261">
         <v>18</v>
@@ -24377,7 +24390,7 @@
         <v>1846.472336890113</v>
       </c>
       <c r="T262">
-        <v>1935.5822101915701</v>
+        <v>1933.758216992019</v>
       </c>
       <c r="V262">
         <v>0</v>
@@ -24463,7 +24476,7 @@
         <v>745.79881894146479</v>
       </c>
       <c r="T263">
-        <v>1738.1834526352279</v>
+        <v>1708.876557123416</v>
       </c>
       <c r="V263">
         <v>27</v>
@@ -25253,7 +25266,7 @@
         <v>1624.4839313243251</v>
       </c>
       <c r="T277">
-        <v>1702.7998658341189</v>
+        <v>1701.196814155669</v>
       </c>
       <c r="V277">
         <v>0</v>
@@ -25348,7 +25361,7 @@
         <v>1643.5171727844711</v>
       </c>
       <c r="T278">
-        <v>1722.75894610604</v>
+        <v>1721.136943399674</v>
       </c>
       <c r="V278">
         <v>0</v>
@@ -25434,7 +25447,7 @@
         <v>1659.2991548039511</v>
       </c>
       <c r="T279">
-        <v>1739.3086055166459</v>
+        <v>1737.670889194168</v>
       </c>
       <c r="V279">
         <v>0</v>
@@ -25520,7 +25533,7 @@
         <v>1687.910531272654</v>
       </c>
       <c r="T280">
-        <v>1769.31174879676</v>
+        <v>1767.645544349394</v>
       </c>
       <c r="V280">
         <v>0</v>
@@ -25606,7 +25619,7 @@
         <v>1705.6461050679429</v>
       </c>
       <c r="T281">
-        <v>1787.91000681931</v>
+        <v>1786.226144057488</v>
       </c>
       <c r="V281">
         <v>0</v>
@@ -25692,7 +25705,7 @@
         <v>1734.5581093459591</v>
       </c>
       <c r="T282">
-        <v>1827.2691373001701</v>
+        <v>1825.3668164913749</v>
       </c>
       <c r="V282">
         <v>0.16666600000000001</v>
@@ -25778,7 +25791,7 @@
         <v>1790.177285774158</v>
       </c>
       <c r="T283">
-        <v>1876.5530619807989</v>
+        <v>1874.7850331129559</v>
       </c>
       <c r="V283">
         <v>0</v>
@@ -25864,7 +25877,7 @@
         <v>1774.203132757508</v>
       </c>
       <c r="T284">
-        <v>1859.801636118576</v>
+        <v>1858.049517276547</v>
       </c>
       <c r="V284">
         <v>0</v>
@@ -26003,7 +26016,7 @@
         <v>1790.277821033746</v>
       </c>
       <c r="T286">
-        <v>1876.6580201481579</v>
+        <v>1874.8899007476559</v>
       </c>
       <c r="V286">
         <v>0</v>
@@ -26089,7 +26102,7 @@
         <v>1846.7213279124001</v>
       </c>
       <c r="T287">
-        <v>1935.846059382219</v>
+        <v>1934.021762050286</v>
       </c>
       <c r="V287">
         <v>0</v>
@@ -26175,7 +26188,7 @@
         <v>1887.1837381913001</v>
       </c>
       <c r="T288">
-        <v>1978.2648632054829</v>
+        <v>1976.4005203837701</v>
       </c>
       <c r="V288">
         <v>0</v>
@@ -26255,7 +26268,7 @@
         <v>1936.0465148686219</v>
       </c>
       <c r="T289">
-        <v>2018.458894723178</v>
+        <v>2016.7719927577259</v>
       </c>
       <c r="V289">
         <v>0</v>
@@ -26344,7 +26357,7 @@
         <v>1692.53446863509</v>
       </c>
       <c r="T290">
-        <v>1774.160803269315</v>
+        <v>1772.48999089173</v>
       </c>
       <c r="V290">
         <v>0</v>
@@ -26439,7 +26452,7 @@
         <v>1976.2127959976849</v>
       </c>
       <c r="T291">
-        <v>2046.4539097812731</v>
+        <v>2045.0161418985069</v>
       </c>
       <c r="V291">
         <v>0</v>
@@ -26525,7 +26538,7 @@
         <v>2028.246540823726</v>
       </c>
       <c r="T292">
-        <v>2087.0838171610631</v>
+        <v>2085.8794748368819</v>
       </c>
       <c r="V292">
         <v>0</v>
@@ -26611,7 +26624,7 @@
         <v>2069.7636911557952</v>
       </c>
       <c r="T293">
-        <v>2116.8484615486459</v>
+        <v>2115.8846816910718</v>
       </c>
       <c r="V293">
         <v>0</v>
@@ -26697,7 +26710,7 @@
         <v>2101.5230534911138</v>
       </c>
       <c r="T294">
-        <v>2138.4083735797799</v>
+        <v>2137.6524488976111</v>
       </c>
       <c r="V294">
         <v>8.3330000000000001E-2</v>
@@ -26780,7 +26793,7 @@
         <v>2140.869307235308</v>
       </c>
       <c r="T295">
-        <v>2164.2671191744112</v>
+        <v>2163.788188520824</v>
       </c>
       <c r="V295">
         <v>0</v>
@@ -26863,7 +26876,7 @@
         <v>2167.9006762585782</v>
       </c>
       <c r="T296">
-        <v>2179.2027863887029</v>
+        <v>2178.97144309021</v>
       </c>
       <c r="V296">
         <v>0</v>
@@ -26946,7 +26959,7 @@
         <v>2189.6376120636392</v>
       </c>
       <c r="T297">
-        <v>2188.6744254123191</v>
+        <v>2188.6941409145052</v>
       </c>
       <c r="V297">
         <v>0</v>
@@ -27029,7 +27042,7 @@
         <v>1641.005942827562</v>
       </c>
       <c r="T298">
-        <v>1720.12561043187</v>
+        <v>1718.50610711182</v>
       </c>
       <c r="V298">
         <v>0</v>
@@ -27124,7 +27137,7 @@
         <v>2103.8971721309581</v>
       </c>
       <c r="T299">
-        <v>2139.0096604480332</v>
+        <v>2138.2909416625962</v>
       </c>
       <c r="V299">
         <v>0</v>
@@ -27269,7 +27282,7 @@
         <v>1709.3548148224349</v>
       </c>
       <c r="T301">
-        <v>1791.7896776915311</v>
+        <v>1790.1023155204459</v>
       </c>
       <c r="V301">
         <v>0</v>
@@ -27367,7 +27380,7 @@
         <v>1715.4354157206419</v>
       </c>
       <c r="T302">
-        <v>1798.1660767239709</v>
+        <v>1796.472659850243</v>
       </c>
       <c r="V302">
         <v>0</v>
@@ -27465,7 +27478,7 @@
         <v>1716.7248157403719</v>
       </c>
       <c r="T303">
-        <v>1799.5182011563861</v>
+        <v>1797.823500374401</v>
       </c>
       <c r="V303">
         <v>0</v>
@@ -27560,7 +27573,7 @@
         <v>1558.7711096394489</v>
       </c>
       <c r="T304">
-        <v>1633.880647300625</v>
+        <v>1632.3432274745201</v>
       </c>
       <c r="V304">
         <v>0</v>
@@ -27646,7 +27659,7 @@
         <v>1600.9662723056031</v>
       </c>
       <c r="T305">
-        <v>1678.1284443361831</v>
+        <v>1676.5490090633909</v>
       </c>
       <c r="V305">
         <v>0</v>
@@ -27732,7 +27745,7 @@
         <v>1586.628124497907</v>
       </c>
       <c r="T306">
-        <v>1667.218584258713</v>
+        <v>1665.5669700790311</v>
       </c>
       <c r="V306">
         <v>8.3330000000000001E-2</v>
@@ -27815,7 +27828,7 @@
         <v>1563.39943378167</v>
       </c>
       <c r="T307">
-        <v>1642.79893554404</v>
+        <v>1641.1717287585259</v>
       </c>
       <c r="V307">
         <v>8.3330000000000001E-2</v>
@@ -27901,7 +27914,7 @@
         <v>1574.9380213794191</v>
       </c>
       <c r="T308">
-        <v>1650.8340178806079</v>
+        <v>1649.280500000239</v>
       </c>
       <c r="V308">
         <v>0</v>
@@ -27987,7 +28000,7 @@
         <v>1639.742100867024</v>
       </c>
       <c r="T309">
-        <v>1718.7905696524469</v>
+        <v>1717.1725237035801</v>
       </c>
       <c r="V309">
         <v>0</v>
@@ -28073,7 +28086,7 @@
         <v>1629.485567675524</v>
       </c>
       <c r="T310">
-        <v>1708.0350950845061</v>
+        <v>1706.427261984607</v>
       </c>
       <c r="V310">
         <v>0</v>
@@ -28159,7 +28172,7 @@
         <v>1607.890345514475</v>
       </c>
       <c r="T311">
-        <v>1685.3893474029519</v>
+        <v>1683.803017547692</v>
       </c>
       <c r="V311">
         <v>0</v>
@@ -28301,7 +28314,7 @@
         <v>1546.75750570325</v>
       </c>
       <c r="T313">
-        <v>1621.2826271711549</v>
+        <v>1619.7571697811161</v>
       </c>
       <c r="V313">
         <v>0</v>
@@ -28387,7 +28400,7 @@
         <v>1767.9260923005029</v>
       </c>
       <c r="T314">
-        <v>1853.210225313728</v>
+        <v>1851.4645413296489</v>
       </c>
       <c r="V314">
         <v>0</v>
@@ -28476,7 +28489,7 @@
         <v>1704.6832984729449</v>
       </c>
       <c r="T315">
-        <v>1786.890909818163</v>
+        <v>1785.2081992666881</v>
       </c>
       <c r="V315">
         <v>0</v>
@@ -28562,7 +28575,7 @@
         <v>1694.5700182475221</v>
       </c>
       <c r="T316">
-        <v>1776.2816725496989</v>
+        <v>1774.6091137607641</v>
       </c>
       <c r="V316">
         <v>0</v>
@@ -28651,7 +28664,7 @@
         <v>1724.9937238653779</v>
       </c>
       <c r="T317">
-        <v>1808.1853758698951</v>
+        <v>1806.4825229547951</v>
       </c>
       <c r="V317">
         <v>0</v>
@@ -28746,7 +28759,7 @@
         <v>2165.2488563747788</v>
       </c>
       <c r="T318">
-        <v>2201.1733459870611</v>
+        <v>2200.438006317926</v>
       </c>
       <c r="V318">
         <v>0</v>
@@ -28832,7 +28845,7 @@
         <v>1748.4243699815911</v>
       </c>
       <c r="T319">
-        <v>1832.7557755718781</v>
+        <v>1831.0295929996639</v>
       </c>
       <c r="V319">
         <v>0</v>
@@ -28918,7 +28931,7 @@
         <v>1746.9972641944671</v>
       </c>
       <c r="T320">
-        <v>1831.2591881720109</v>
+        <v>1829.534427821425</v>
       </c>
       <c r="V320">
         <v>0</v>
@@ -29004,7 +29017,7 @@
         <v>1774.1683946368089</v>
       </c>
       <c r="T321">
-        <v>1859.7520199231949</v>
+        <v>1858.000205621011</v>
       </c>
       <c r="V321">
         <v>0</v>
@@ -29090,7 +29103,7 @@
         <v>1769.958966346042</v>
       </c>
       <c r="T322">
-        <v>1855.3378189371899</v>
+        <v>1853.5901961346649</v>
       </c>
       <c r="V322">
         <v>0</v>
@@ -29229,7 +29242,7 @@
         <v>1790.0259091369519</v>
       </c>
       <c r="T324">
-        <v>1876.380854073494</v>
+        <v>1874.6132516016669</v>
       </c>
       <c r="V324">
         <v>0</v>
@@ -29315,7 +29328,7 @@
         <v>1809.4325302466621</v>
       </c>
       <c r="T325">
-        <v>1896.731421040346</v>
+        <v>1894.9444969068411</v>
       </c>
       <c r="V325">
         <v>0</v>
@@ -29401,7 +29414,7 @@
         <v>1826.0638806416689</v>
       </c>
       <c r="T326">
-        <v>1914.1716748871031</v>
+        <v>1912.368193279769</v>
       </c>
       <c r="V326">
         <v>0</v>
@@ -29487,7 +29500,7 @@
         <v>1849.042918441058</v>
       </c>
       <c r="T327">
-        <v>1938.268350415977</v>
+        <v>1936.4419918417859</v>
       </c>
       <c r="V327">
         <v>0</v>
@@ -29573,7 +29586,7 @@
         <v>1877.3881717422321</v>
       </c>
       <c r="T328">
-        <v>1967.992190935526</v>
+        <v>1966.1376140100101</v>
       </c>
       <c r="V328">
         <v>0</v>
@@ -29659,7 +29672,7 @@
         <v>1894.21050808775</v>
       </c>
       <c r="T329">
-        <v>1985.632382914345</v>
+        <v>1983.761065272475</v>
       </c>
       <c r="V329">
         <v>0</v>
@@ -29798,7 +29811,7 @@
         <v>2212.639032777849</v>
       </c>
       <c r="T331">
-        <v>2230.4051451229102</v>
+        <v>2230.041489930738</v>
       </c>
       <c r="V331">
         <v>0</v>
@@ -29884,7 +29897,7 @@
         <v>1930.0120487798849</v>
       </c>
       <c r="T332">
-        <v>2023.172230653397</v>
+        <v>2021.2653315421021</v>
       </c>
       <c r="V332">
         <v>0</v>
@@ -29970,7 +29983,7 @@
         <v>1968.2979738928691</v>
       </c>
       <c r="T333">
-        <v>2057.9045481577982</v>
+        <v>2056.0703879683729</v>
       </c>
       <c r="V333">
         <v>0</v>
@@ -30050,7 +30063,7 @@
         <v>2024.659005245207</v>
       </c>
       <c r="T334">
-        <v>2102.640534262659</v>
+        <v>2101.0443275422522</v>
       </c>
       <c r="V334">
         <v>0</v>
@@ -30136,7 +30149,7 @@
         <v>2064.2871208534712</v>
       </c>
       <c r="T335">
-        <v>2130.0264592800322</v>
+        <v>2128.68083839886</v>
       </c>
       <c r="V335">
         <v>0</v>
@@ -30222,7 +30235,7 @@
         <v>2115.250497478326</v>
       </c>
       <c r="T336">
-        <v>2169.47076222134</v>
+        <v>2168.3609256734362</v>
       </c>
       <c r="V336">
         <v>0</v>
@@ -30308,7 +30321,7 @@
         <v>2144.387705854283</v>
       </c>
       <c r="T337">
-        <v>2186.1743367849499</v>
+        <v>2185.3190047344619</v>
       </c>
       <c r="V337">
         <v>0</v>
@@ -30391,7 +30404,7 @@
         <v>2242.4890594860199</v>
       </c>
       <c r="T338">
-        <v>2241.4541382243342</v>
+        <v>2241.4753220648381</v>
       </c>
       <c r="V338">
         <v>0</v>
@@ -30474,7 +30487,7 @@
         <v>1725.606445971222</v>
       </c>
       <c r="T339">
-        <v>1808.8279045785321</v>
+        <v>1807.124441551008</v>
       </c>
       <c r="V339">
         <v>0</v>

</xml_diff>